<commit_message>
Updates for phs000465, 468, 469
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000465_Diagnos-ActeMyelLeuk_SampleAnatcSite-Blood-StudyStatus.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000465_Diagnos-ActeMyelLeuk_SampleAnatcSite-Blood-StudyStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBDCCA-2072-45D8-8486-2158E98377E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AA3BCA-BBEB-4E49-865A-69FCC169FBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="500" yWindow="-26660" windowWidth="35140" windowHeight="20160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,25 +63,6 @@
   </si>
   <si>
     <t>StudiesTab</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT prt.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT cmf.id)) AS "Files"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-Left JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"     
-LEFT JOIN 
-    df_clinical_measure_file cmf ON std.id = cmf."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000465' and dgn.diagnosis = 'Acute Myeloid Leukemia, NOS' and smp.anatomic_site = 'C42.0 : Blood' and std.study_status = 'Completed' ;</t>
   </si>
   <si>
     <t>TC01_CCDI_phs000465_Diagnos-ActeLeukOfAmbigLinge_DiagAnatSite-Blood_WebData.xlsx</t>
@@ -204,129 +185,362 @@
 LEFT JOIN funding fd ON s.study_id = fd.study_id;  -- Changed alias from 'f' to 'fd' here</t>
   </si>
   <si>
-    <t>with file_data as (
-select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
-SELECT fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type" ,
-        CASE     
-    WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        END
-    WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        END
-    WHEN fd.file_size &gt;= 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-            ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-        END
-    ELSE 
-        CASE 
-            WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-            ELSE ROUND(fd.file_size, 2) || ' Bytes'
-        END
-END AS "File Size",
-fd.file_access AS "File Access", std.dbgap_accession AS "Study ID", fd.participantid AS "Participant ID", null as "Sample ID"
-FROM 
-    df_study std
- LEFT JOIN  
-    file_data fd ON std.id = fd.studyid
-WHERE 
-    std.dbgap_accession = 'phs000465'</t>
-  </si>
-  <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ) 
+    <t>TC01_CCDI_phs000465_Diagnos-ActeMyelLeuk_SampleAnatcSite-Blood-StudyStatus_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>WITH diag_base AS (
+  SELECT DISTINCT
+    d."participant.id"        AS participant_id,
+    d.age_at_diagnosis        AS age_at_diagnosis,
+    d.diagnosis               AS diagnosis,
+    d.anatomic_site           AS anatomic_site,
+    d.diagnosis_category      AS diagnosis_category
+  FROM df_diagnosis d
+  WHERE d."participant.id" IS NOT NULL
+),
+diagnosis_summary AS (
+  SELECT
+    participant_id,
+    /* normalize -999 before concatenating */
+    GROUP_CONCAT(
+      CASE
+        WHEN age_at_diagnosis = '-999' THEN 'Not Reported'
+        ELSE age_at_diagnosis
+      END,
+      ';'
+    )                                      AS age_at_diagnosis,
+    GROUP_CONCAT(diagnosis, ';')           AS diagnosis,
+    GROUP_CONCAT(anatomic_site, ';')       AS anatomic_site,
+    GROUP_CONCAT(diagnosis_category, ';')  AS diagnosis_category
+  FROM diag_base
+  GROUP BY participant_id
+),
+surv_base AS (
+  SELECT DISTINCT
+    s."participant.id"           AS participant_id,
+    s.last_known_survival_status AS last_known_survival_status
+  FROM df_survival s
+),
+survival_summary AS (
+  SELECT
+    participant_id,
+    GROUP_CONCAT(last_known_survival_status, ';') AS last_known_survival_status
+  FROM surv_base
+  GROUP BY participant_id
+)
+/* final select */
+SELECT
+  prt.participant_id                           AS "Participant ID",
+  std.dbgap_accession                          AS "Study ID",
+  COALESCE(prt.sex_at_birth, '')               AS "Sex",
+  COALESCE(prt.race, '')                       AS "Race",
+  COALESCE(dsum.diagnosis, '')                 AS "Diagnosis",
+  COALESCE(dsum.anatomic_site, '')             AS "Diagnosis Anatomic Site",
+  COALESCE(dsum.diagnosis_category, '')        AS "Diagnosis_Category",
+  COALESCE(dsum.age_at_diagnosis, '')          AS "Age at Diagnosis (days)",
+  NULL                                         AS "Treatment Type",
+  COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
+FROM df_study std
+LEFT JOIN df_consent_group    cg   ON std.id = cg."study.id"
+LEFT JOIN df_participant      prt  ON cg.id  = prt."consent_group.id"
+LEFT JOIN diagnosis_summary   dsum ON prt.id = dsum.participant_id
+LEFT JOIN survival_summary    srv  ON prt.id = srv.participant_id
+WHERE
+  std.dbgap_accession = 'phs000465'
+  AND std.study_status LIKE 'Completed%'
+  /* apply TC01 filters */
+  AND EXISTS (
+    SELECT 1
+    FROM df_diagnosis d
+    WHERE d."participant.id" = prt.id
+      AND d.diagnosis        LIKE 'Acute Myeloid Leukemia%'
+  )
+  AND EXISTS (
+    SELECT 1
+    FROM df_sample sm
+    WHERE sm."participant.id" = prt.id
+      AND sm.anatomic_site    LIKE '%Blood%'
+  )
+ORDER BY prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH qualified_participants AS (
+  /* participants that match study/status + AML + Blood */
+  SELECT DISTINCT prt.id AS participant_row_id
+  FROM df_study std
+  JOIN df_consent_group cg
+    ON std.id = cg."study.id"
+  JOIN df_participant prt
+    ON cg.id = prt."consent_group.id"
+  WHERE
+    std.dbgap_accession = 'phs000465'
+    AND std.study_status LIKE 'Completed%'
+    AND EXISTS (
+      SELECT 1
+      FROM df_diagnosis d
+      WHERE d."participant.id" = prt.id
+        AND d.diagnosis        LIKE 'Acute Myeloid Leukemia%'
+    )
+    AND EXISTS (
+      SELECT 1
+      FROM df_sample sm_check
+      WHERE sm_check."participant.id" = prt.id
+        AND sm_check.anatomic_site    LIKE '%Blood%'
+    )
+),
+qualified_samples AS (
+  SELECT DISTINCT sm.sample_id
+  FROM df_sample sm
+  WHERE
+    sm."participant.id" IN (SELECT participant_row_id FROM qualified_participants)
+    AND sm.anatomic_site LIKE '%Blood%'
+),
+files_base AS (
+  SELECT
+    cmf.id                AS file_row_id,
+    cmf."study.id"        AS study_row_id,
+    cmf."participant.id"  AS participant_row_id
+  FROM df_clinical_measure_file cmf
+),
+qualified_files AS (
+  SELECT DISTINCT fb.file_row_id
+  FROM files_base fb
+  JOIN df_study std
+    ON fb.study_row_id = std.id
+  WHERE
+    std.dbgap_accession = 'phs000465'
+    AND std.study_status LIKE 'Completed%'
+    AND (
+      fb.participant_row_id IS NULL
+      OR fb.participant_row_id = ''
+      OR fb.participant_row_id IN (
+        SELECT participant_row_id
+        FROM qualified_participants
+      )
+    )
+),
+qualified_studies AS (
+  SELECT DISTINCT std.dbgap_accession AS study_accession
+  FROM df_study std
+  WHERE
+    std.dbgap_accession = 'phs000465'
+    AND std.study_status LIKE 'Completed%'
+)
+SELECT
+  /* Studies count */
+  (SELECT COUNT(DISTINCT study_accession) FROM qualified_studies)    AS "Studies",
+  /* Participants count */
+  (SELECT COUNT(DISTINCT participant_row_id) FROM qualified_participants) AS "Participants",
+  /* Samples count */
+  (SELECT COUNT(DISTINCT sample_id) FROM qualified_samples)          AS "Samples",
+  /* Files count */
+  (SELECT COUNT(DISTINCT file_row_id) FROM qualified_files)          AS "Files";</t>
+  </si>
+  <si>
+    <t>WITH cg_map AS (
+  SELECT
+    id         AS consent_row_id,
+    "study.id" AS study_row_id
+  FROM df_consent_group
+),
+prt AS (
+  SELECT
+    p.participant_id,
+    p.id           AS participant_row_id,
+    cg.study_row_id
+  FROM df_participant p
+  JOIN cg_map cg
+    ON cg.consent_row_id = p."consent_group.id"
+),
+smp AS (
+  SELECT
+    s.sample_id,
+    COALESCE(s.anatomic_site, '') AS sample_anatomic_site,
+    CASE
+      WHEN COALESCE(CAST(s.participant_age_at_collection AS TEXT), '') IN ('', '-999')
+        THEN 'Not Reported'
+      ELSE CAST(s.participant_age_at_collection AS TEXT)
+    END AS age_at_collection_days,
+    CASE
+      WHEN TRIM(COALESCE(s.sample_tumor_status, '')) = '' THEN 'Not Reported'
+      ELSE s.sample_tumor_status
+    END AS sample_tumor_status,
+    CASE
+      WHEN TRIM(COALESCE(s.tumor_classification, '')) = '' THEN 'Not Reported'
+      ELSE s.tumor_classification
+    END AS sample_tumor_classification,
+    s.id               AS sample_row_id,
+    s."participant.id" AS participant_row_id,
+    UPPER(TRIM(COALESCE(s.anatomic_site, ''))) AS anatomic_site_u
+  FROM df_sample s
+),
+-- SAMPLE-LEVEL diagnosis only (no participant fallback)
+diag_s_names AS (
+  SELECT y."sample.id" AS sample_row_id,
+         GROUP_CONCAT(y.diagnosis, ';') AS sample_diag
+  FROM (
+    SELECT DISTINCT
+      "sample.id",
+      COALESCE(diagnosis, '') AS diagnosis
+    FROM df_diagnosis
+    WHERE "sample.id" IS NOT NULL
+  ) y
+  GROUP BY y."sample.id"
+),
+diag_s_cat AS (
+  SELECT y."sample.id" AS sample_row_id,
+         GROUP_CONCAT(y.diagnosis_category, ';') AS sample_diag_cat
+  FROM (
+    SELECT DISTINCT
+      "sample.id",
+      COALESCE(diagnosis_category, '') AS diagnosis_category
+    FROM df_diagnosis
+    WHERE "sample.id" IS NOT NULL
+  ) y
+  GROUP BY y."sample.id"
+),
+-- AML filter helper (participant has AML diagnosis)
+aml_participants AS (
+  SELECT DISTINCT d."participant.id" AS participant_row_id
+  FROM df_diagnosis d
+  WHERE UPPER(TRIM(COALESCE(d.diagnosis,''))) LIKE 'ACUTE MYELOID LEUKEMIA%'
+)
 SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-Left Join
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs000465' and dgn.diagnosis = 'Acute Myeloid Leukemia, NOS' and smp.anatomic_site = 'C42.0 : Blood' and std.study_status = 'Completed'
-ORDER BY 
-    prt.participant_id ASC limit 100;</t>
-  </si>
-  <si>
-    <t>TC01_CCDI_phs000465_Diagnos-ActeMyelLeuk_SampleAnatcSite-Blood-StudyStatus_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    COALESCE(
-        CASE 
-            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' 
-            ELSE smp.participant_age_at_collection 
-        END, 
-        0
-    ) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    CASE 
-        WHEN dgn."sample.id" IS NOT NULL THEN dgn.diagnosis
-        ELSE NULL
-    END AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs000465' 
-    AND dgn.diagnosis = 'Acute Myeloid Leukemia, NOS' 
-    AND smp.anatomic_site = 'C42.0 : Blood' 
-    AND std.study_status = 'Completed'
-    AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC;</t>
+  smp.sample_id                                   AS "Sample ID",
+  prt.participant_id                              AS "Participant ID",
+  std.dbgap_accession                             AS "Study ID",
+  smp.sample_anatomic_site                        AS "Sample Anatomic Site",
+  smp.age_at_collection_days                      AS "Age at Sample Collection (days)",
+  smp.sample_tumor_status                         AS "Sample Tumor Status",
+  smp.sample_tumor_classification                 AS "Sample Tumor Classification",
+  COALESCE(dsn.sample_diag, '')                   AS "Sample Diagnosis",
+  COALESCE(dsc.sample_diag_cat, '')               AS "Diagnosis Category"
+FROM df_study std
+JOIN prt
+  ON std.id = prt.study_row_id
+JOIN smp
+  ON smp.participant_row_id = prt.participant_row_id
+JOIN aml_participants aml
+  ON aml.participant_row_id = prt.participant_row_id
+LEFT JOIN diag_s_names dsn
+  ON dsn.sample_row_id = smp.sample_row_id
+LEFT JOIN diag_s_cat dsc
+  ON dsc.sample_row_id = smp.sample_row_id
+WHERE UPPER(TRIM(std.dbgap_accession)) LIKE UPPER(TRIM('phs000465%'))
+  AND UPPER(TRIM(COALESCE(std.study_status,''))) LIKE 'COMPLETED%'
+  AND smp.anatomic_site_u LIKE '%BLOOD%'
+  AND smp.sample_id IS NOT NULL
+ORDER BY smp.sample_id ASC;</t>
+  </si>
+  <si>
+    <t>WITH cg_map AS (
+  SELECT id AS consent_row_id, "study.id" AS study_row_id
+  FROM df_consent_group
+),
+-- Cohort: participants in phs000465 / Completed% with AML dx and a Blood sample
+qualified_participants AS (
+  SELECT DISTINCT p.id AS participant_row_id
+  FROM df_study std
+  JOIN cg_map cg
+    ON std.id = cg.study_row_id
+  JOIN df_participant p
+    ON p."consent_group.id" = cg.consent_row_id
+  WHERE UPPER(TRIM(COALESCE(std.dbgap_accession,''))) LIKE 'PHS000465%'
+    AND UPPER(TRIM(COALESCE(std.study_status,''))) LIKE 'COMPLETED%'
+    AND EXISTS (
+      SELECT 1
+      FROM df_diagnosis d
+      WHERE d."participant.id" = p.id
+        AND UPPER(TRIM(COALESCE(d.diagnosis,''))) LIKE 'ACUTE MYELOID LEUKEMIA%'
+    )
+    AND EXISTS (
+      SELECT 1
+      FROM df_sample s
+      WHERE s."participant.id" = p.id
+        AND UPPER(TRIM(COALESCE(s.anatomic_site,''))) LIKE '%BLOOD%'
+    )
+),
+-- Files table with clean aliases and pre-normalized category
+cmf AS (
+  SELECT
+    clinical_measure_file_id,
+    file_name,
+    REPLACE(COALESCE(data_category, ''), ';', ', ') AS data_category,
+    COALESCE(file_description, '')                  AS file_description,
+    COALESCE(file_type, '')                         AS file_type,
+    COALESCE(file_access, '')                       AS file_access,
+    COALESCE(file_size, 0)                          AS file_size,
+    "study.id"                                      AS study_row_id,
+    "participant.id"                                AS participant_row_id
+  FROM df_clinical_measure_file
+)
+SELECT DISTINCT
+  cmf.file_name AS "File Name",
+  cmf.data_category AS "Data Category",
+  cmf.file_description AS "File Description",
+  cmf.file_type AS "File Type",
+  CASE
+    WHEN cmf.file_size &gt;= 1024 * 1024 * 1024 THEN
+      CASE WHEN ROUND(cmf.file_size / (1024.0 * 1024.0 * 1024.0), 2)
+                 = CAST(ROUND(cmf.file_size / (1024.0 * 1024.0 * 1024.0), 2) AS INTEGER)
+           THEN CAST(ROUND(cmf.file_size / (1024.0 * 1024.0 * 1024.0), 2) AS INTEGER) || ' GB'
+           ELSE ROUND(cmf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' END
+    WHEN cmf.file_size &gt;= 1024 * 1024 THEN
+      CASE WHEN ROUND(cmf.file_size / (1024.0 * 1024.0), 2)
+                 = CAST(ROUND(cmf.file_size / (1024.0 * 1024.0), 2) AS INTEGER)
+           THEN CAST(ROUND(cmf.file_size / (1024.0 * 1024.0), 2) AS INTEGER) || ' MB'
+           ELSE ROUND(cmf.file_size / (1024.0 * 1024.0), 2) || ' MB' END
+    WHEN cmf.file_size &gt;= 1024 THEN
+      CASE WHEN ROUND(cmf.file_size / 1024.0, 2)
+                 = CAST(ROUND(cmf.file_size / 1024.0, 2) AS INTEGER)
+           THEN CAST(ROUND(cmf.file_size / 1024.0, 2) AS INTEGER) || ' KB'
+           ELSE ROUND(cmf.file_size / 1024.0, 2) || ' KB' END
+    ELSE CAST(cmf.file_size AS TEXT) || ' B'
+  END AS "File Size",
+  cmf.file_access AS "Access",
+  std.dbgap_accession AS "Study ID",
+  -- UI convention: keep blank for study-level files
+  CASE WHEN cmf.participant_row_id IS NULL THEN '' ELSE COALESCE(p.participant_id,'') END AS "Participant ID",
+  '' AS "Sample ID"   -- keep blank to avoid row-multiplying joins; add if UI truly shows sample ids for file rows
+FROM df_study std
+JOIN cmf
+  ON cmf.study_row_id = std.id
+LEFT JOIN df_participant p
+  ON p.id = cmf.participant_row_id
+WHERE UPPER(TRIM(std.dbgap_accession)) LIKE 'PHS000465%'
+  AND UPPER(TRIM(COALESCE(std.study_status,''))) LIKE 'COMPLETED%'
+  -- keep pure study-level files OR files tied to a qualified participant
+  AND (
+       cmf.participant_row_id IS NULL
+    OR cmf.participant_row_id IN (SELECT participant_row_id FROM qualified_participants)
+  )
+  -- ensure we’re in the cohort context (at least one qualified participant exists)
+  AND EXISTS (SELECT 1 FROM qualified_participants)
+ORDER BY cmf.file_name ASC;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -386,14 +600,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -719,19 +939,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="47.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -748,58 +968,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="355.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="355" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>